<commit_message>
implement function qlRelinkableHandleLinkTo() and implement coercion in function qlTermStructureReferenceDate()
</commit_message>
<xml_diff>
--- a/Data2/XLS/EUR/EUR_MainChecks.xlsx
+++ b/Data2/XLS/EUR/EUR_MainChecks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="60">
   <si>
     <t>ObjectID</t>
   </si>
@@ -784,39 +784,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
-<volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <volType type="realTimeData">
-    <main first="pldatasource.rdatartdserver">
-      <tp t="s">
-        <v>Updated at 15:21:51</v>
-        <stp/>
-        <stp>{113A892D-4CD1-497F-B308-AA8CDA15A9EB}</stp>
-        <tr r="Q5" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 15:21:29</v>
-        <stp/>
-        <stp>{352F2324-65C4-4828-AF5D-EC90C2899719}</stp>
-        <tr r="Q6" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 15:21:35</v>
-        <stp/>
-        <stp>{2CF6BBB2-90CB-473F-9E14-D20AAA4FD6E8}</stp>
-        <tr r="P7" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 15:21:35</v>
-        <stp/>
-        <stp>{BC086328-803A-407B-9494-67FD453A7587}</stp>
-        <tr r="Q7" s="2"/>
-      </tp>
-    </main>
-  </volType>
-</volTypes>
-</file>
-
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
@@ -1205,7 +1172,7 @@
   <dimension ref="A1:AJ104"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="11.25" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -1296,7 +1263,9 @@
       <c r="T2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="18"/>
+      <c r="U2" s="18">
+        <v>42242.044652777775</v>
+      </c>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
@@ -1463,9 +1432,9 @@
       <c r="N5" s="26"/>
       <c r="O5" s="26"/>
       <c r="P5" s="26"/>
-      <c r="Q5" s="27" t="str">
-        <f>_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
-        <v>Updated at 15:21:51</v>
+      <c r="Q5" s="27" t="e">
+        <f ca="1">_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
+        <v>#NAME?</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>13</v>
@@ -1476,7 +1445,7 @@
       </c>
       <c r="U5" s="11" t="str">
         <f>_xll.ohBoostVersion(Trigger)&amp;" / "&amp;_xll.ohVersion(Trigger)&amp;" / "&amp;_xll.qlVersion(Trigger)</f>
-        <v>1_52 / 1.5.0 / 1.5</v>
+        <v>1_52 / 1.6.0 / 1.6.2</v>
       </c>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
@@ -1533,9 +1502,9 @@
       <c r="N6" s="28"/>
       <c r="O6" s="28"/>
       <c r="P6" s="28"/>
-      <c r="Q6" s="29" t="str">
-        <f>_xll.RData(K6,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L6)</f>
-        <v>Updated at 15:21:29</v>
+      <c r="Q6" s="29" t="e">
+        <f ca="1">_xll.RData(K6,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L6)</f>
+        <v>#NAME?</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>13</v>
@@ -1546,7 +1515,7 @@
       </c>
       <c r="U6" s="11">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>2934</v>
+        <v>1332</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1608,13 +1577,13 @@
       <c r="O7" s="28">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P7" s="28" t="str">
-        <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N7)</f>
-        <v>Updated at 15:21:35</v>
-      </c>
-      <c r="Q7" s="29" t="str">
-        <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L7)</f>
-        <v>Updated at 15:21:35</v>
+      <c r="P7" s="28" t="e">
+        <f ca="1">_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N7)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="Q7" s="29" t="e">
+        <f ca="1">_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L7)</f>
+        <v>#NAME?</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>13</v>
@@ -1791,20 +1760,20 @@
         <f>PROPER(Currency)&amp;VLOOKUP(Currency,FuturesTable,8,0)&amp;VLOOKUP(Currency,FuturesTable,2,0)</f>
         <v>Euribor6M</v>
       </c>
-      <c r="L10" s="25">
-        <f>_xll.qlCalendarAdvance("TARGET",L11,"-1M","f",,Trigger)</f>
-        <v>41904</v>
-      </c>
-      <c r="M10" s="58">
-        <f>_xll.qlIndexFixing(FirstIndex,L10,,Trigger)</f>
-        <v>1.8599999999999999E-3</v>
+      <c r="L10" s="25" t="e">
+        <f ca="1">_xll.qlCalendarAdvance("TARGET",L11,"-1M","f",,Trigger)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M10" s="58" t="e">
+        <f ca="1">_xll.qlIndexFixing(FirstIndex,L10,,Trigger)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="N10" s="58"/>
       <c r="O10" s="58"/>
       <c r="P10" s="58"/>
       <c r="Q10" s="59" t="str">
-        <f>IF(AND(ISERROR(L10),ISERROR(M10)),_xll.ohRangeRetrieveError(L10)&amp;" "&amp;_xll.ohRangeRetrieveError(M10),IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10)))</f>
-        <v/>
+        <f ca="1">IF(AND(ISERROR(L10),ISERROR(M10)),_xll.ohRangeRetrieveError(L10)&amp;" "&amp;_xll.ohRangeRetrieveError(M10),IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10)))</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="R10" s="8" t="s">
         <v>13</v>
@@ -1856,20 +1825,20 @@
       <c r="I11" s="3"/>
       <c r="J11" s="7"/>
       <c r="K11" s="39"/>
-      <c r="L11" s="40">
-        <f>_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>41932</v>
-      </c>
-      <c r="M11" s="60">
+      <c r="L11" s="40" t="e">
+        <f ca="1">_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M11" s="60" t="e">
         <f>_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>1.8400000000000001E-3</v>
+        <v>#NUM!</v>
       </c>
       <c r="N11" s="60"/>
       <c r="O11" s="60"/>
       <c r="P11" s="60"/>
       <c r="Q11" s="61" t="str">
-        <f>IF(AND(ISERROR(L11),ISERROR(M11)),_xll.ohRangeRetrieveError(L11)&amp;" "&amp;_xll.ohRangeRetrieveError(M11),IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11)))</f>
-        <v/>
+        <f ca="1">IF(AND(ISERROR(L11),ISERROR(M11)),_xll.ohRangeRetrieveError(L11)&amp;" "&amp;_xll.ohRangeRetrieveError(M11),IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11)))</f>
+        <v xml:space="preserve"> qlQuoteValue - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0446527778'</v>
       </c>
       <c r="R11" s="8"/>
       <c r="S11" s="1"/>
@@ -1917,23 +1886,21 @@
         <v>EURSTD</v>
       </c>
       <c r="L12" s="22">
-        <f>_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
-        <v>41932</v>
-      </c>
-      <c r="M12" s="23">
-        <f>_xll.qlYieldTSDiscount(K12,L12)</f>
-        <v>1</v>
+        <f>_xll.qlTermStructureReferenceDate(Trigger,K12)</f>
+        <v>42242</v>
+      </c>
+      <c r="M12" s="23" t="e">
+        <f>_xll.qlYieldTermStructureDiscount(,K12,L12)</f>
+        <v>#NUM!</v>
       </c>
       <c r="N12" s="23"/>
       <c r="O12" s="23"/>
       <c r="P12" s="23"/>
       <c r="Q12" s="31" t="str">
-        <f>IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
-        <v/>
-      </c>
-      <c r="R12" s="8" t="s">
-        <v>13</v>
-      </c>
+        <f ca="1">IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
+        <v>qlYieldTermStructureDiscount - Error retrieving object with id 'EURSTD' - unable to convert reference to type 'class QuantLibAddin::YieldTermStructure' found instead 'class QuantLibAddin::RelinkableHandleYieldTermStructure'</v>
+      </c>
+      <c r="R12" s="8"/>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
@@ -1968,20 +1935,20 @@
         <f>UPPER(Currency)&amp;"ON"</f>
         <v>EURON</v>
       </c>
-      <c r="L13" s="22">
+      <c r="L13" s="22" t="e">
         <f>_xll.qlTermStructureReferenceDate(K13,Trigger)</f>
-        <v>41932</v>
-      </c>
-      <c r="M13" s="23">
-        <f>_xll.qlYieldTSDiscount(K13,L13)</f>
-        <v>1</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="M13" s="23" t="e">
+        <f ca="1">_xll.qlYieldTSDiscount(K13,L13)</f>
+        <v>#NAME?</v>
       </c>
       <c r="N13" s="23"/>
       <c r="O13" s="23"/>
       <c r="P13" s="23"/>
       <c r="Q13" s="31" t="str">
-        <f>IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
-        <v/>
+        <f ca="1">IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
+        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0446527778'</v>
       </c>
       <c r="R13" s="8" t="s">
         <v>13</v>
@@ -2010,13 +1977,13 @@
       <c r="B14" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="C14" s="33">
+      <c r="C14" s="33" t="e">
         <f t="array" ref="C14:C17">_xll.qlIMMNextDates(_xll.qlSettingsEvaluationDate(Trigger)-1,B14:B17)</f>
-        <v>41990</v>
-      </c>
-      <c r="D14" s="6" t="str">
+        <v>#NUM!</v>
+      </c>
+      <c r="D14" s="6" t="e">
         <f t="array" ref="D14:D17">VLOOKUP(Currency,FuturesTable,4,0)&amp;_xll.qlIMMcode(FuturesDates)</f>
-        <v>FEIZ4</v>
+        <v>#NUM!</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -2028,20 +1995,20 @@
         <f>UPPER(Currency)&amp;"1M"</f>
         <v>EUR1M</v>
       </c>
-      <c r="L14" s="22">
+      <c r="L14" s="22" t="e">
         <f>_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
-        <v>41934</v>
-      </c>
-      <c r="M14" s="23">
-        <f>_xll.qlYieldTSDiscount(K14,L14)</f>
-        <v>1</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="M14" s="23" t="e">
+        <f ca="1">_xll.qlYieldTSDiscount(K14,L14)</f>
+        <v>#NAME?</v>
       </c>
       <c r="N14" s="23"/>
       <c r="O14" s="23"/>
       <c r="P14" s="23"/>
       <c r="Q14" s="32" t="str">
-        <f>IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
-        <v/>
+        <f ca="1">IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
+        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0446527778'</v>
       </c>
       <c r="R14" s="8" t="s">
         <v>13</v>
@@ -2070,11 +2037,11 @@
       <c r="B15" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="C15" s="34">
-        <v>42081</v>
-      </c>
-      <c r="D15" s="8" t="str">
-        <v>FEIH5</v>
+      <c r="C15" s="34" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="D15" s="8" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -2086,20 +2053,20 @@
         <f>UPPER(Currency)&amp;"3M"</f>
         <v>EUR3M</v>
       </c>
-      <c r="L15" s="22">
+      <c r="L15" s="22" t="e">
         <f>_xll.qlTermStructureReferenceDate(K15,Trigger)</f>
-        <v>41934</v>
-      </c>
-      <c r="M15" s="23">
-        <f>_xll.qlYieldTSDiscount(K15,L15)</f>
-        <v>1</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="M15" s="23" t="e">
+        <f ca="1">_xll.qlYieldTSDiscount(K15,L15)</f>
+        <v>#NAME?</v>
       </c>
       <c r="N15" s="23"/>
       <c r="O15" s="23"/>
       <c r="P15" s="23"/>
       <c r="Q15" s="32" t="str">
-        <f>IF(ISERROR(L15),_xll.ohRangeRetrieveError(L15),_xll.ohRangeRetrieveError(M15))</f>
-        <v/>
+        <f ca="1">IF(ISERROR(L15),_xll.ohRangeRetrieveError(L15),_xll.ohRangeRetrieveError(M15))</f>
+        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0446527778'</v>
       </c>
       <c r="R15" s="8" t="s">
         <v>13</v>
@@ -2128,11 +2095,11 @@
       <c r="B16" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="C16" s="34">
-        <v>42172</v>
-      </c>
-      <c r="D16" s="8" t="str">
-        <v>FEIM5</v>
+      <c r="C16" s="34" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="D16" s="8" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -2144,20 +2111,20 @@
         <f>UPPER(Currency)&amp;"6M"</f>
         <v>EUR6M</v>
       </c>
-      <c r="L16" s="22">
+      <c r="L16" s="22" t="e">
         <f>_xll.qlTermStructureReferenceDate(K16,Trigger)</f>
-        <v>41934</v>
-      </c>
-      <c r="M16" s="23">
-        <f>_xll.qlYieldTSDiscount(K16,L16)</f>
-        <v>1</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="M16" s="23" t="e">
+        <f ca="1">_xll.qlYieldTSDiscount(K16,L16)</f>
+        <v>#NAME?</v>
       </c>
       <c r="N16" s="23"/>
       <c r="O16" s="23"/>
       <c r="P16" s="23"/>
       <c r="Q16" s="32" t="str">
-        <f>IF(ISERROR(L16),_xll.ohRangeRetrieveError(L16),_xll.ohRangeRetrieveError(M16))</f>
-        <v/>
+        <f ca="1">IF(ISERROR(L16),_xll.ohRangeRetrieveError(L16),_xll.ohRangeRetrieveError(M16))</f>
+        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0446527778'</v>
       </c>
       <c r="R16" s="8" t="s">
         <v>13</v>
@@ -2186,11 +2153,11 @@
       <c r="B17" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="C17" s="35">
-        <v>42263</v>
-      </c>
-      <c r="D17" s="10" t="str">
-        <v>FEIU5</v>
+      <c r="C17" s="35" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="D17" s="10" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -2202,20 +2169,20 @@
         <f>UPPER(Currency)&amp;"1Y"</f>
         <v>EUR1Y</v>
       </c>
-      <c r="L17" s="40">
+      <c r="L17" s="40" t="e">
         <f>_xll.qlTermStructureReferenceDate(K17,Trigger)</f>
-        <v>41934</v>
-      </c>
-      <c r="M17" s="41">
-        <f>_xll.qlYieldTSDiscount(K17,L17)</f>
-        <v>1</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="M17" s="41" t="e">
+        <f ca="1">_xll.qlYieldTSDiscount(K17,L17)</f>
+        <v>#NAME?</v>
       </c>
       <c r="N17" s="41"/>
       <c r="O17" s="41"/>
       <c r="P17" s="41"/>
       <c r="Q17" s="42" t="str">
-        <f>IF(ISERROR(L17),_xll.ohRangeRetrieveError(L17),_xll.ohRangeRetrieveError(M17))</f>
-        <v/>
+        <f ca="1">IF(ISERROR(L17),_xll.ohRangeRetrieveError(L17),_xll.ohRangeRetrieveError(M17))</f>
+        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0446527778'</v>
       </c>
       <c r="R17" s="8" t="s">
         <v>13</v>
@@ -2258,15 +2225,15 @@
         <v>#NUM!</v>
       </c>
       <c r="M18" s="55" t="e">
-        <f>_xll.qlYieldTSDiscount(K18,L18)</f>
-        <v>#NUM!</v>
+        <f ca="1">_xll.qlYieldTSDiscount(K18,L18)</f>
+        <v>#NAME?</v>
       </c>
       <c r="N18" s="55"/>
       <c r="O18" s="55"/>
       <c r="P18" s="55"/>
       <c r="Q18" s="56" t="str">
         <f ca="1">IF(ISERROR(L18),_xll.ohRangeRetrieveError(L18),_xll.ohRangeRetrieveError(M18))</f>
-        <v/>
+        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0446527778'</v>
       </c>
       <c r="R18" s="8" t="s">
         <v>13</v>
@@ -2309,15 +2276,15 @@
         <v>#NUM!</v>
       </c>
       <c r="M19" s="41" t="e">
-        <f>_xll.qlYieldTSDiscount(K19,L19)</f>
-        <v>#NUM!</v>
+        <f ca="1">_xll.qlYieldTSDiscount(K19,L19)</f>
+        <v>#NAME?</v>
       </c>
       <c r="N19" s="41"/>
       <c r="O19" s="41"/>
       <c r="P19" s="41"/>
       <c r="Q19" s="42" t="str">
         <f ca="1">IF(ISERROR(L19),_xll.ohRangeRetrieveError(L19),_xll.ohRangeRetrieveError(M19))</f>
-        <v/>
+        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0446527778'</v>
       </c>
       <c r="R19" s="8" t="s">
         <v>13</v>
@@ -5485,7 +5452,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="CommandButton1">
+        <control shapeId="1026" r:id="rId4" name="CommandButton2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5505,12 +5472,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="CommandButton1"/>
+        <control shapeId="1026" r:id="rId4" name="CommandButton2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId6" name="CommandButton2">
+        <control shapeId="1025" r:id="rId6" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5530,7 +5497,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId6" name="CommandButton2"/>
+        <control shapeId="1025" r:id="rId6" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
fix coercion in function qlYieldTermStructureDiscount()
</commit_message>
<xml_diff>
--- a/Data2/XLS/EUR/EUR_MainChecks.xlsx
+++ b/Data2/XLS/EUR/EUR_MainChecks.xlsx
@@ -1264,7 +1264,7 @@
         <v>1</v>
       </c>
       <c r="U2" s="18">
-        <v>42242.044652777775</v>
+        <v>42242.057199074072</v>
       </c>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
@@ -1826,7 +1826,7 @@
       <c r="J11" s="7"/>
       <c r="K11" s="39"/>
       <c r="L11" s="40" t="e">
-        <f ca="1">_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <f ca="1">qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
         <v>#NAME?</v>
       </c>
       <c r="M11" s="60" t="e">
@@ -1838,7 +1838,7 @@
       <c r="P11" s="60"/>
       <c r="Q11" s="61" t="str">
         <f ca="1">IF(AND(ISERROR(L11),ISERROR(M11)),_xll.ohRangeRetrieveError(L11)&amp;" "&amp;_xll.ohRangeRetrieveError(M11),IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11)))</f>
-        <v xml:space="preserve"> qlQuoteValue - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0446527778'</v>
+        <v xml:space="preserve"> qlQuoteValue - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0571990741'</v>
       </c>
       <c r="R11" s="8"/>
       <c r="S11" s="1"/>
@@ -1889,16 +1889,16 @@
         <f>_xll.qlTermStructureReferenceDate(Trigger,K12)</f>
         <v>42242</v>
       </c>
-      <c r="M12" s="23" t="e">
+      <c r="M12" s="23">
         <f>_xll.qlYieldTermStructureDiscount(,K12,L12)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="N12" s="23"/>
       <c r="O12" s="23"/>
       <c r="P12" s="23"/>
       <c r="Q12" s="31" t="str">
-        <f ca="1">IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
-        <v>qlYieldTermStructureDiscount - Error retrieving object with id 'EURSTD' - unable to convert reference to type 'class QuantLibAddin::YieldTermStructure' found instead 'class QuantLibAddin::RelinkableHandleYieldTermStructure'</v>
+        <f>IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
+        <v/>
       </c>
       <c r="R12" s="8"/>
       <c r="S12" s="1"/>
@@ -1948,7 +1948,7 @@
       <c r="P13" s="23"/>
       <c r="Q13" s="31" t="str">
         <f ca="1">IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
-        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0446527778'</v>
+        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0571990741'</v>
       </c>
       <c r="R13" s="8" t="s">
         <v>13</v>
@@ -2008,7 +2008,7 @@
       <c r="P14" s="23"/>
       <c r="Q14" s="32" t="str">
         <f ca="1">IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
-        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0446527778'</v>
+        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0571990741'</v>
       </c>
       <c r="R14" s="8" t="s">
         <v>13</v>
@@ -2066,7 +2066,7 @@
       <c r="P15" s="23"/>
       <c r="Q15" s="32" t="str">
         <f ca="1">IF(ISERROR(L15),_xll.ohRangeRetrieveError(L15),_xll.ohRangeRetrieveError(M15))</f>
-        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0446527778'</v>
+        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0571990741'</v>
       </c>
       <c r="R15" s="8" t="s">
         <v>13</v>
@@ -2124,7 +2124,7 @@
       <c r="P16" s="23"/>
       <c r="Q16" s="32" t="str">
         <f ca="1">IF(ISERROR(L16),_xll.ohRangeRetrieveError(L16),_xll.ohRangeRetrieveError(M16))</f>
-        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0446527778'</v>
+        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0571990741'</v>
       </c>
       <c r="R16" s="8" t="s">
         <v>13</v>
@@ -2182,7 +2182,7 @@
       <c r="P17" s="41"/>
       <c r="Q17" s="42" t="str">
         <f ca="1">IF(ISERROR(L17),_xll.ohRangeRetrieveError(L17),_xll.ohRangeRetrieveError(M17))</f>
-        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0446527778'</v>
+        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0571990741'</v>
       </c>
       <c r="R17" s="8" t="s">
         <v>13</v>
@@ -2233,7 +2233,7 @@
       <c r="P18" s="55"/>
       <c r="Q18" s="56" t="str">
         <f ca="1">IF(ISERROR(L18),_xll.ohRangeRetrieveError(L18),_xll.ohRangeRetrieveError(M18))</f>
-        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0446527778'</v>
+        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0571990741'</v>
       </c>
       <c r="R18" s="8" t="s">
         <v>13</v>
@@ -2284,7 +2284,7 @@
       <c r="P19" s="41"/>
       <c r="Q19" s="42" t="str">
         <f ca="1">IF(ISERROR(L19),_xll.ohRangeRetrieveError(L19),_xll.ohRangeRetrieveError(M19))</f>
-        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0446527778'</v>
+        <v>qlTermStructureReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID '42242.0571990741'</v>
       </c>
       <c r="R19" s="8" t="s">
         <v>13</v>
@@ -5452,7 +5452,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId4" name="CommandButton2">
+        <control shapeId="1025" r:id="rId4" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5472,12 +5472,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId4" name="CommandButton2"/>
+        <control shapeId="1025" r:id="rId4" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId6" name="CommandButton1">
+        <control shapeId="1026" r:id="rId6" name="CommandButton2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5497,7 +5497,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId6" name="CommandButton1"/>
+        <control shapeId="1026" r:id="rId6" name="CommandButton2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>